<commit_message>
temp excel: row from 1
</commit_message>
<xml_diff>
--- a/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ExcelTemplate/SMS/SMS_DanhSachTinNhan_Template.xlsx
+++ b/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ExcelTemplate/SMS/SMS_DanhSachTinNhan_Template.xlsx
@@ -32,25 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>HoTen</t>
-  </si>
-  <si>
-    <t>NgaySinh</t>
-  </si>
-  <si>
-    <t>SoDienThoai</t>
-  </si>
-  <si>
-    <t>TenTinhThanh</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>NgayBatDauLamViec</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>DANH SÁCH TIN NHẮN ĐÃ GỬI</t>
   </si>
@@ -543,12 +525,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CJ86"/>
+  <dimension ref="A1:CJ85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,172 +547,193 @@
     <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:88" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="6"/>
+      <c r="AM2" s="6"/>
+      <c r="AN2" s="6"/>
+      <c r="AO2" s="6"/>
+      <c r="AP2" s="6"/>
+    </row>
+    <row r="3" spans="1:88" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C3" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="E3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:88" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="J3" s="5"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="6"/>
-      <c r="AL3" s="6"/>
-      <c r="AM3" s="6"/>
-      <c r="AN3" s="6"/>
-      <c r="AO3" s="6"/>
-      <c r="AP3" s="6"/>
-    </row>
-    <row r="4" spans="1:88" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="11"/>
-      <c r="AI4" s="11"/>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="11"/>
-      <c r="AL4" s="11"/>
-      <c r="AM4" s="11"/>
-      <c r="AN4" s="11"/>
-      <c r="AO4" s="11"/>
-      <c r="AP4" s="11"/>
-      <c r="AQ4" s="11"/>
-      <c r="AR4" s="11"/>
-      <c r="AS4" s="11"/>
-      <c r="AT4" s="11"/>
-      <c r="AU4" s="11"/>
-      <c r="AV4" s="11"/>
-      <c r="AW4" s="11"/>
-      <c r="AX4" s="11"/>
-      <c r="AY4" s="11"/>
-      <c r="AZ4" s="11"/>
-      <c r="BA4" s="11"/>
-      <c r="BB4" s="11"/>
-      <c r="BC4" s="11"/>
-      <c r="BD4" s="11"/>
-      <c r="BE4" s="11"/>
-      <c r="BF4" s="11"/>
-      <c r="BG4" s="11"/>
-      <c r="BH4" s="11"/>
-      <c r="BI4" s="11"/>
-      <c r="BJ4" s="11"/>
-      <c r="BK4" s="11"/>
-      <c r="BL4" s="11"/>
-      <c r="BM4" s="11"/>
-      <c r="BN4" s="11"/>
-      <c r="BO4" s="11"/>
-      <c r="BP4" s="11"/>
-      <c r="BQ4" s="11"/>
-      <c r="BR4" s="11"/>
-      <c r="BS4" s="11"/>
-      <c r="BT4" s="11"/>
-      <c r="BU4" s="11"/>
-      <c r="BV4" s="11"/>
-      <c r="BW4" s="11"/>
-      <c r="BX4" s="11"/>
-      <c r="BY4" s="11"/>
-      <c r="BZ4" s="11"/>
-      <c r="CA4" s="11"/>
-      <c r="CB4" s="11"/>
-      <c r="CC4" s="11"/>
-      <c r="CD4" s="11"/>
-      <c r="CE4" s="11"/>
-      <c r="CF4" s="11"/>
-      <c r="CG4" s="11"/>
-      <c r="CH4" s="11"/>
-      <c r="CI4" s="11"/>
-      <c r="CJ4" s="11"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="11"/>
+      <c r="AI3" s="11"/>
+      <c r="AJ3" s="11"/>
+      <c r="AK3" s="11"/>
+      <c r="AL3" s="11"/>
+      <c r="AM3" s="11"/>
+      <c r="AN3" s="11"/>
+      <c r="AO3" s="11"/>
+      <c r="AP3" s="11"/>
+      <c r="AQ3" s="11"/>
+      <c r="AR3" s="11"/>
+      <c r="AS3" s="11"/>
+      <c r="AT3" s="11"/>
+      <c r="AU3" s="11"/>
+      <c r="AV3" s="11"/>
+      <c r="AW3" s="11"/>
+      <c r="AX3" s="11"/>
+      <c r="AY3" s="11"/>
+      <c r="AZ3" s="11"/>
+      <c r="BA3" s="11"/>
+      <c r="BB3" s="11"/>
+      <c r="BC3" s="11"/>
+      <c r="BD3" s="11"/>
+      <c r="BE3" s="11"/>
+      <c r="BF3" s="11"/>
+      <c r="BG3" s="11"/>
+      <c r="BH3" s="11"/>
+      <c r="BI3" s="11"/>
+      <c r="BJ3" s="11"/>
+      <c r="BK3" s="11"/>
+      <c r="BL3" s="11"/>
+      <c r="BM3" s="11"/>
+      <c r="BN3" s="11"/>
+      <c r="BO3" s="11"/>
+      <c r="BP3" s="11"/>
+      <c r="BQ3" s="11"/>
+      <c r="BR3" s="11"/>
+      <c r="BS3" s="11"/>
+      <c r="BT3" s="11"/>
+      <c r="BU3" s="11"/>
+      <c r="BV3" s="11"/>
+      <c r="BW3" s="11"/>
+      <c r="BX3" s="11"/>
+      <c r="BY3" s="11"/>
+      <c r="BZ3" s="11"/>
+      <c r="CA3" s="11"/>
+      <c r="CB3" s="11"/>
+      <c r="CC3" s="11"/>
+      <c r="CD3" s="11"/>
+      <c r="CE3" s="11"/>
+      <c r="CF3" s="11"/>
+      <c r="CG3" s="11"/>
+      <c r="CH3" s="11"/>
+      <c r="CI3" s="11"/>
+      <c r="CJ3" s="11"/>
+    </row>
+    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="6"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
     </row>
     <row r="5" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
@@ -852,8 +855,6 @@
       <c r="AL7" s="6"/>
       <c r="AM7" s="6"/>
       <c r="AN7" s="6"/>
-      <c r="AO7" s="6"/>
-      <c r="AP7" s="6"/>
     </row>
     <row r="8" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
@@ -1096,37 +1097,6 @@
       <c r="D14" s="19"/>
       <c r="E14" s="22"/>
       <c r="F14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="6"/>
-      <c r="AH14" s="6"/>
-      <c r="AI14" s="6"/>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="6"/>
-      <c r="AL14" s="6"/>
-      <c r="AM14" s="6"/>
-      <c r="AN14" s="6"/>
     </row>
     <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
@@ -1137,11 +1107,11 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="22"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1696,17 +1666,9 @@
       <c r="E85" s="23"/>
       <c r="F85" s="5"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="16"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="20"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="23"/>
-      <c r="F86" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>